<commit_message>
LaTex: fixed ALK, added some parameters in Tables, FORTRAN + MATLAB: played with SWI-fluxes
</commit_message>
<xml_diff>
--- a/CHECK_SWI-FLUX_O2_TOC_Int_0102.xlsx
+++ b/CHECK_SWI-FLUX_O2_TOC_Int_0102.xlsx
@@ -16,12 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
-  <si>
-    <t>Exp below with zbio=10cm, so TOC degradation in bioturbated and non-bioturbated layer. </t>
-  </si>
-  <si>
-    <t>There is just a tiny tiny change for the integrated TOC degradation rates with changing k-values left (2nd and 3rd column below). This also causes an equivalent difference in O2-SWI-flux (4th and 5th column). </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+  <si>
+    <t>Exp below with zbio=10cm, so TOC degradation in bioturbated and non-bioturbated layer.</t>
+  </si>
+  <si>
+    <t>There is just a tiny tiny change for the integrated TOC degradation rates with changing k-values left (2nd and 3rd column below). This also causes an equivalent difference in O2-SWI-flux (4th and 5th column).</t>
   </si>
   <si>
     <t>I also compared the calculated O2-flux with the theoretical O2-demand (6th column). The values are also very similar and approach the theoretical value for higher k (7th and 8th column).</t>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>K=2.0</t>
+  </si>
+  <si>
+    <t>K=3.0</t>
   </si>
   <si>
     <t>ALL NON-Bioturbated</t>
@@ -342,7 +345,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -484,6 +487,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -604,15 +611,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1785714285714"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4642857142857"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0561224489796"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.1020408163265"/>
@@ -732,14 +739,14 @@
         <v>2.65441224306622E-005</v>
       </c>
       <c r="C8" s="19" t="n">
-        <f aca="false">B8/B$41</f>
+        <f aca="false">B8/B$46</f>
         <v>1</v>
       </c>
       <c r="D8" s="18" t="n">
         <v>-7.27193507624543E-006</v>
       </c>
       <c r="E8" s="19" t="n">
-        <f aca="false">D8/D$41</f>
+        <f aca="false">D8/D$46</f>
         <v>0.913188358394717</v>
       </c>
       <c r="F8" s="18" t="n">
@@ -765,14 +772,14 @@
         <v>2.64257505291113E-005</v>
       </c>
       <c r="C9" s="19" t="n">
-        <f aca="false">B9/B$41</f>
+        <f aca="false">B9/B$46</f>
         <v>0.995540560745223</v>
       </c>
       <c r="D9" s="18" t="n">
         <v>-7.9277251587334E-006</v>
       </c>
       <c r="E9" s="19" t="n">
-        <f aca="false">D9/D$41</f>
+        <f aca="false">D9/D$46</f>
         <v>0.995540560745225</v>
       </c>
       <c r="F9" s="18" t="n">
@@ -808,14 +815,14 @@
         <v>2.64421673928606E-005</v>
       </c>
       <c r="C10" s="19" t="n">
-        <f aca="false">B10/B$41</f>
+        <f aca="false">B10/B$46</f>
         <v>0.996159035279169</v>
       </c>
       <c r="D10" s="18" t="n">
         <v>-7.93265021785814E-006</v>
       </c>
       <c r="E10" s="19" t="n">
-        <f aca="false">D10/D$41</f>
+        <f aca="false">D10/D$46</f>
         <v>0.996159035279165</v>
       </c>
       <c r="F10" s="18" t="n">
@@ -851,14 +858,14 @@
         <v>2.65429217454686E-005</v>
       </c>
       <c r="C11" s="19" t="n">
-        <f aca="false">B11/B$41</f>
+        <f aca="false">B11/B$46</f>
         <v>0.999954766438531</v>
       </c>
       <c r="D11" s="18" t="n">
         <v>-7.96287652363969E-006</v>
       </c>
       <c r="E11" s="19" t="n">
-        <f aca="false">D11/D$41</f>
+        <f aca="false">D11/D$46</f>
         <v>0.999954766438421</v>
       </c>
       <c r="F11" s="18" t="n">
@@ -894,14 +901,14 @@
         <v>2.65440672602384E-005</v>
       </c>
       <c r="C12" s="30" t="n">
-        <f aca="false">B12/B$41</f>
+        <f aca="false">B12/B$46</f>
         <v>0.999997921557816</v>
       </c>
       <c r="D12" s="29" t="n">
         <v>-7.96322017808089E-006</v>
       </c>
       <c r="E12" s="30" t="n">
-        <f aca="false">D12/D$41</f>
+        <f aca="false">D12/D$46</f>
         <v>0.999997921558994</v>
       </c>
       <c r="F12" s="29" t="n">
@@ -937,14 +944,14 @@
         <v>2.65441216170908E-005</v>
       </c>
       <c r="C13" s="19" t="n">
-        <f aca="false">B13/B$41</f>
+        <f aca="false">B13/B$46</f>
         <v>0.999999969350224</v>
       </c>
       <c r="D13" s="29" t="n">
         <v>-7.96323648496311E-006</v>
       </c>
       <c r="E13" s="19" t="n">
-        <f aca="false">D13/D$41</f>
+        <f aca="false">D13/D$46</f>
         <v>0.999999969329614</v>
       </c>
       <c r="F13" s="29" t="n">
@@ -974,12 +981,15 @@
         <v>28</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="36"/>
+    </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="6"/>
       <c r="E16" s="8"/>
     </row>
@@ -1013,7 +1023,7 @@
       <c r="D18" s="18" t="n">
         <v>-4.93651134775928E-006</v>
       </c>
-      <c r="E18" s="37" t="n">
+      <c r="E18" s="38" t="n">
         <v>-5.51088399591927E-022</v>
       </c>
     </row>
@@ -1030,7 +1040,7 @@
       <c r="D19" s="18" t="n">
         <v>-2.23142971782911E-007</v>
       </c>
-      <c r="E19" s="37" t="n">
+      <c r="E19" s="38" t="n">
         <v>-6.70802246041072E-167</v>
       </c>
     </row>
@@ -1047,7 +1057,7 @@
       <c r="D20" s="18" t="n">
         <v>-3.62307952543332E-025</v>
       </c>
-      <c r="E20" s="37" t="n">
+      <c r="E20" s="38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1064,7 +1074,7 @@
       <c r="D21" s="18" t="n">
         <v>-6.80416815252049E-169</v>
       </c>
-      <c r="E21" s="37" t="n">
+      <c r="E21" s="38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1081,7 +1091,7 @@
       <c r="D22" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="E22" s="37" t="n">
+      <c r="E22" s="38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1089,16 +1099,16 @@
       <c r="A23" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="38" t="n">
+      <c r="C23" s="39" t="n">
         <v>-8.13571432445315E-013</v>
       </c>
-      <c r="D23" s="38" t="n">
+      <c r="D23" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="E23" s="39" t="n">
+      <c r="E23" s="40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1109,23 +1119,23 @@
       <c r="C26" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="40" t="n">
+      <c r="D26" s="41" t="n">
         <v>-7.94547266840715E-006</v>
       </c>
       <c r="E26" s="0" t="n">
-        <f aca="false">D26/D$41</f>
+        <f aca="false">D26/D$46</f>
         <v>0.99776924115211</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="40" t="n">
+      <c r="D27" s="41" t="n">
         <v>-7.96322845363977E-006</v>
       </c>
       <c r="E27" s="0" t="n">
-        <f aca="false">D27/D$41</f>
+        <f aca="false">D27/D$46</f>
         <v>0.999998960779497</v>
       </c>
     </row>
@@ -1133,11 +1143,23 @@
       <c r="A30" s="35" t="s">
         <v>39</v>
       </c>
+      <c r="B30" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="24" t="s">
         <v>40</v>
       </c>
+      <c r="B31" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -1157,35 +1179,33 @@
       <c r="B33" s="2" t="n">
         <v>2.65441224306622E-005</v>
       </c>
+      <c r="C33" s="36"/>
       <c r="D33" s="2" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="F33" s="40" t="n">
-        <v>6.16865194287026E-006</v>
-      </c>
-      <c r="G33" s="40"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
       <c r="H33" s="0" t="n">
         <f aca="false">-F33/D32</f>
-        <v>0.774641286281466</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="42" t="n">
+      <c r="B34" s="43" t="n">
         <v>-268435455.999973</v>
       </c>
       <c r="D34" s="2" t="n">
         <v>-7.96323672919865E-006</v>
       </c>
-      <c r="F34" s="40" t="n">
-        <v>1.14774912588703E-007</v>
-      </c>
-      <c r="G34" s="40"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
       <c r="H34" s="0" t="n">
         <f aca="false">-F34/D33</f>
-        <v>0.0144130981523957</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,24 +1218,33 @@
       <c r="D35" s="2" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="F35" s="2" t="n">
-        <v>-7.96323672919866E-006</v>
-      </c>
+      <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="43" t="n">
+      <c r="H35" s="44" t="n">
         <f aca="false">-F35/D34</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="44" t="n">
+      <c r="B36" s="45" t="n">
         <v>-2.12676479325586E+037</v>
       </c>
-      <c r="D36" s="44" t="n">
+      <c r="D36" s="45" t="n">
         <v>5.51765372175541E+036</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="36" t="n">
+        <v>2.65441224306622E-005</v>
+      </c>
+      <c r="D37" s="36" t="n">
+        <v>-7.96323672919866E-006</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1228,94 +1257,106 @@
       <c r="H38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="2" t="n">
-        <v>2.65441224306622E-005</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>-7.96323672919865E-006</v>
-      </c>
       <c r="E41" s="18"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="2" t="n">
-        <v>2.65441224306622E-005</v>
-      </c>
-      <c r="D42" s="2" t="n">
-        <v>-7.96323672919865E-006</v>
-      </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="2" t="n">
-        <v>2.65441224306622E-005</v>
-      </c>
-      <c r="D43" s="2" t="n">
-        <v>-7.96323672919865E-006</v>
-      </c>
-      <c r="E43" s="45"/>
+      <c r="E43" s="46"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="2" t="n">
-        <v>2.65441224306622E-005</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>-7.96323672919865E-006</v>
-      </c>
+      <c r="A44" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>2.65441224306622E-005</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>-7.96323672919865E-006</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>2.65441224306622E-005</v>
+      </c>
+      <c r="C47" s="36"/>
+      <c r="D47" s="2" t="n">
+        <v>-7.96323672919865E-006</v>
+      </c>
+      <c r="E47" s="36"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>2.65441224306622E-005</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>-7.96323672919865E-006</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>2.65441224306622E-005</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>-7.96323672919865E-006</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="2" t="n">
+      <c r="B50" s="2" t="n">
         <v>2.65441224306622E-005</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D50" s="2" t="n">
         <v>-7.96323672919865E-006</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fortran: added subroutine for 2nd diffusion coefficient; TeX: changed SWI_flux calculation and minor things
</commit_message>
<xml_diff>
--- a/CHECK_SWI-FLUX_O2_TOC_Int_0102.xlsx
+++ b/CHECK_SWI-FLUX_O2_TOC_Int_0102.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="433" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="433" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="1 diff coeff" sheetId="1" state="visible" r:id="rId2"/>
@@ -281,7 +281,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="14">
+  <numFmts count="15">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.0000000E+000"/>
@@ -293,9 +293,10 @@
     <numFmt numFmtId="172" formatCode="0.000000E+000"/>
     <numFmt numFmtId="173" formatCode="0.0000E+000"/>
     <numFmt numFmtId="174" formatCode="0.000000000"/>
-    <numFmt numFmtId="175" formatCode="0.000"/>
-    <numFmt numFmtId="176" formatCode="0.0000"/>
-    <numFmt numFmtId="177" formatCode="0.00000000E+000"/>
+    <numFmt numFmtId="175" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="0.0000"/>
+    <numFmt numFmtId="178" formatCode="0.00000000E+000"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -504,7 +505,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -785,6 +786,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -821,19 +826,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="173" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -914,10 +919,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2063,6 +2068,24 @@
       </c>
       <c r="D61" s="2" t="n">
         <v>-7.96323672919865E-006</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="50"/>
+      <c r="C68" s="50" t="n">
+        <v>-7.96323672919866E-006</v>
+      </c>
+      <c r="D68" s="50" t="n">
+        <v>-7.96323507297679E-006</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="50"/>
+      <c r="C69" s="70" t="n">
+        <v>-7.96323672919689E-006</v>
+      </c>
+      <c r="D69" s="50" t="n">
+        <v>-7.96323672943744E-006</v>
       </c>
     </row>
   </sheetData>
@@ -2207,7 +2230,7 @@
       <c r="F8" s="29" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="G8" s="70" t="n">
+      <c r="G8" s="71" t="n">
         <f aca="false">D8/F8</f>
         <v>-0</v>
       </c>
@@ -2238,7 +2261,7 @@
       <c r="F9" s="29" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="G9" s="70" t="n">
+      <c r="G9" s="71" t="n">
         <f aca="false">D9/F9</f>
         <v>1.00223824488279</v>
       </c>
@@ -2246,7 +2269,7 @@
         <f aca="false">D9-F9</f>
         <v>-1.78236738595918E-008</v>
       </c>
-      <c r="I9" s="71" t="n">
+      <c r="I9" s="72" t="n">
         <v>1.44959E-038</v>
       </c>
     </row>
@@ -2271,7 +2294,7 @@
       <c r="F10" s="29" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="G10" s="70" t="n">
+      <c r="G10" s="71" t="n">
         <f aca="false">D10/F10</f>
         <v>1.00000158064292</v>
       </c>
@@ -2279,7 +2302,7 @@
         <f aca="false">D10-F10</f>
         <v>-1.25870337813934E-011</v>
       </c>
-      <c r="I10" s="71" t="n">
+      <c r="I10" s="72" t="n">
         <v>2.00389E-088</v>
       </c>
     </row>
@@ -2304,7 +2327,7 @@
       <c r="F11" s="39" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="G11" s="72" t="n">
+      <c r="G11" s="73" t="n">
         <f aca="false">D11/F11</f>
         <v>1.00000000544705</v>
       </c>
@@ -2312,7 +2335,7 @@
         <f aca="false">D11-F11</f>
         <v>-4.33761709818688E-014</v>
       </c>
-      <c r="I11" s="71" t="n">
+      <c r="I11" s="72" t="n">
         <v>8.31613E-126</v>
       </c>
     </row>
@@ -2337,7 +2360,7 @@
       <c r="F12" s="44" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="G12" s="73" t="n">
+      <c r="G12" s="74" t="n">
         <f aca="false">D12/F12</f>
         <v>0.999999177492195</v>
       </c>
@@ -2345,7 +2368,7 @@
         <f aca="false">D12-F12</f>
         <v>6.54982435950298E-012</v>
       </c>
-      <c r="I12" s="74" t="n">
+      <c r="I12" s="75" t="n">
         <v>7.24195E-180</v>
       </c>
     </row>
@@ -2442,7 +2465,7 @@
       <c r="F19" s="29" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="G19" s="70" t="n">
+      <c r="G19" s="71" t="n">
         <f aca="false">D19/F19</f>
         <v>1.00377703586994</v>
       </c>
@@ -2475,7 +2498,7 @@
       <c r="F20" s="29" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="G20" s="70" t="n">
+      <c r="G20" s="71" t="n">
         <f aca="false">D20/F20</f>
         <v>1.00073402761177</v>
       </c>
@@ -2483,7 +2506,7 @@
         <f aca="false">D20-F20</f>
         <v>-5.84523563826123E-009</v>
       </c>
-      <c r="I20" s="71" t="n">
+      <c r="I20" s="72" t="n">
         <v>1.10231E-103</v>
       </c>
     </row>
@@ -2508,7 +2531,7 @@
       <c r="F21" s="29" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="G21" s="70" t="n">
+      <c r="G21" s="71" t="n">
         <f aca="false">D21/F21</f>
         <v>0.999738200749237</v>
       </c>
@@ -2516,7 +2539,7 @@
         <f aca="false">D21-F21</f>
         <v>2.08476940934949E-009</v>
       </c>
-      <c r="I21" s="71" t="n">
+      <c r="I21" s="72" t="n">
         <v>5.94743E-267</v>
       </c>
     </row>
@@ -2541,7 +2564,7 @@
       <c r="F22" s="39" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="G22" s="72" t="n">
+      <c r="G22" s="73" t="n">
         <f aca="false">D22/F22</f>
         <v>0.999983416386614</v>
       </c>
@@ -2549,7 +2572,7 @@
         <f aca="false">D22-F22</f>
         <v>1.32059239218773E-010</v>
       </c>
-      <c r="I22" s="75" t="n">
+      <c r="I22" s="76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2574,7 +2597,7 @@
       <c r="F23" s="44" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
-      <c r="G23" s="73" t="n">
+      <c r="G23" s="74" t="n">
         <f aca="false">D23/F23</f>
         <v>0.999999660401919</v>
       </c>
@@ -2582,7 +2605,7 @@
         <f aca="false">D23-F23</f>
         <v>2.70429991029405E-012</v>
       </c>
-      <c r="I23" s="75" t="n">
+      <c r="I23" s="76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2693,7 +2716,7 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -2713,22 +2736,22 @@
       <c r="A1" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="78" t="n">
+      <c r="C2" s="79" t="n">
         <v>-7.96323672919866E-006</v>
       </c>
       <c r="D2" s="11" t="n">
@@ -2751,7 +2774,7 @@
       <c r="F3" s="15" t="n">
         <v>0.1</v>
       </c>
-      <c r="G3" s="79" t="n">
+      <c r="G3" s="80" t="n">
         <v>0.001</v>
       </c>
     </row>
@@ -2771,7 +2794,7 @@
       <c r="F4" s="50" t="n">
         <v>1.10231E-103</v>
       </c>
-      <c r="G4" s="80" t="n">
+      <c r="G4" s="81" t="n">
         <v>0.000948483</v>
       </c>
     </row>
@@ -2841,19 +2864,19 @@
       <c r="B8" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="81" t="n">
+      <c r="C8" s="82" t="n">
         <f aca="false">+C5/$C$2-1</f>
         <v>2.9985569582891E-011</v>
       </c>
-      <c r="D8" s="81" t="n">
+      <c r="D8" s="82" t="n">
         <f aca="false">+D5/$C$2-1</f>
         <v>2.40883846203133E-009</v>
       </c>
-      <c r="E8" s="81" t="n">
+      <c r="E8" s="82" t="n">
         <f aca="false">+E5/$C$2-1</f>
         <v>5.581160953394E-007</v>
       </c>
-      <c r="F8" s="81" t="n">
+      <c r="F8" s="82" t="n">
         <f aca="false">+F5/$C$2-1</f>
         <v>0.000734029993604057</v>
       </c>
@@ -2868,10 +2891,10 @@
       <c r="D9" s="50" t="n">
         <v>-4.40261327394609E-010</v>
       </c>
-      <c r="E9" s="82" t="n">
+      <c r="E9" s="83" t="n">
         <v>-6.96404606898016E-009</v>
       </c>
-      <c r="F9" s="82" t="n">
+      <c r="F9" s="83" t="n">
         <v>-2.96685276295408E-007</v>
       </c>
       <c r="G9" s="50" t="n">
@@ -2888,10 +2911,10 @@
       <c r="D10" s="50" t="n">
         <v>-4.40261404542198E-010</v>
       </c>
-      <c r="E10" s="82" t="n">
+      <c r="E10" s="83" t="n">
         <v>-6.96404606697194E-009</v>
       </c>
-      <c r="F10" s="82" t="n">
+      <c r="F10" s="83" t="n">
         <v>-2.96685276295345E-007</v>
       </c>
       <c r="G10" s="50" t="n">
@@ -2965,19 +2988,19 @@
       <c r="B14" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="81" t="n">
+      <c r="C14" s="82" t="n">
         <f aca="false">+C12/$D$2-1</f>
         <v>5.45503642257472E-011</v>
       </c>
-      <c r="D14" s="81" t="n">
+      <c r="D14" s="82" t="n">
         <f aca="false">+D12/$D$2-1</f>
         <v>2.40901520953685E-009</v>
       </c>
-      <c r="E14" s="81" t="n">
+      <c r="E14" s="82" t="n">
         <f aca="false">+E12/$D$2-1</f>
         <v>5.58115926807545E-007</v>
       </c>
-      <c r="F14" s="81" t="n">
+      <c r="F14" s="82" t="n">
         <f aca="false">+F12/$D$2-1</f>
         <v>0.000734029993603613</v>
       </c>
@@ -2986,22 +3009,22 @@
       <c r="A18" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76" t="s">
+      <c r="B18" s="77"/>
+      <c r="C18" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="76" t="s">
+      <c r="D18" s="77" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="78" t="n">
+      <c r="C19" s="79" t="n">
         <v>-2.58899747288259E-006</v>
       </c>
       <c r="D19" s="11" t="n">
@@ -3024,7 +3047,7 @@
       <c r="F20" s="15" t="n">
         <v>0.1</v>
       </c>
-      <c r="G20" s="79" t="n">
+      <c r="G20" s="80" t="n">
         <v>0.001</v>
       </c>
     </row>
@@ -3038,7 +3061,7 @@
       <c r="D21" s="50"/>
       <c r="E21" s="50"/>
       <c r="F21" s="50"/>
-      <c r="G21" s="80"/>
+      <c r="G21" s="81"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="15" t="s">
@@ -3106,23 +3129,23 @@
       <c r="B25" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="81" t="n">
+      <c r="C25" s="82" t="n">
         <f aca="false">+C22/$C$2-1</f>
         <v>-0.674821989701321</v>
       </c>
-      <c r="D25" s="81" t="n">
+      <c r="D25" s="82" t="n">
         <f aca="false">+D22/$C$2-1</f>
         <v>-1</v>
       </c>
-      <c r="E25" s="81" t="n">
+      <c r="E25" s="82" t="n">
         <f aca="false">+E22/$C$2-1</f>
         <v>-1</v>
       </c>
-      <c r="F25" s="81" t="n">
+      <c r="F25" s="82" t="n">
         <f aca="false">+F22/$C$2-1</f>
         <v>-1</v>
       </c>
-      <c r="G25" s="81" t="n">
+      <c r="G25" s="82" t="n">
         <f aca="false">+G22/$C$2-1</f>
         <v>-1</v>
       </c>
@@ -3135,8 +3158,8 @@
         <v>-1.13938647907451E-007</v>
       </c>
       <c r="D26" s="50"/>
-      <c r="E26" s="82"/>
-      <c r="F26" s="82"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
       <c r="G26" s="50"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3147,8 +3170,8 @@
         <v>-1.13938647907469E-007</v>
       </c>
       <c r="D27" s="50"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="82"/>
+      <c r="E27" s="83"/>
+      <c r="F27" s="83"/>
       <c r="G27" s="50"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3210,25 +3233,25 @@
       <c r="B31" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="81" t="n">
+      <c r="C31" s="82" t="n">
         <f aca="false">+C29/$D$2-1</f>
         <v>-1</v>
       </c>
-      <c r="D31" s="81" t="n">
+      <c r="D31" s="82" t="n">
         <f aca="false">+D29/$D$2-1</f>
         <v>-1</v>
       </c>
-      <c r="E31" s="81" t="n">
+      <c r="E31" s="82" t="n">
         <f aca="false">+E29/$D$2-1</f>
         <v>-1</v>
       </c>
-      <c r="F31" s="81" t="n">
+      <c r="F31" s="82" t="n">
         <f aca="false">+F29/$D$2-1</f>
         <v>-1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="77" t="s">
+      <c r="A35" s="78" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>